<commit_message>
added new methods - RequisitioningPage,MainNavPage added new sheet under catalog
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/Catalog.xlsx
+++ b/src/test/resources/datasheets/Catalog.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14985" windowHeight="6210"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14985" windowHeight="6210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SmartForm" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="VerifyCatalogSearch" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Role</t>
   </si>
@@ -63,6 +63,33 @@
   </si>
   <si>
     <t>EA-EACH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CatalogSearchInput </t>
+  </si>
+  <si>
+    <t>LocalSearch</t>
+  </si>
+  <si>
+    <t>GlobalSearch</t>
+  </si>
+  <si>
+    <t>BPO</t>
+  </si>
+  <si>
+    <t>MAGNA DECOPLAS</t>
+  </si>
+  <si>
+    <t>COMPUTER DESKTOP</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>global</t>
+  </si>
+  <si>
+    <t>bpo</t>
   </si>
 </sst>
 </file>
@@ -894,7 +921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -976,12 +1003,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1. Developed a new test in catalog Module - TC07_Add_PriceAgreementItem_RecentOrder. 2. Created two new page classes - RecentOrderInformationPage & ItemDetailsPage. 3. Added the following methods in Recent Order and ItemDetaislpage classes:     - clickCartItemsLink,clickItemNumberLink & selectUOMValueAndAddItemToCart.
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/Catalog.xlsx
+++ b/src/test/resources/datasheets/Catalog.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14985" windowHeight="6210"/>
+    <workbookView xWindow="600" yWindow="4230" windowWidth="19320" windowHeight="6015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SmartForm" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="AddPriceAgreement" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
+  <oleSize ref="A1:S18"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Role</t>
   </si>
@@ -63,6 +64,12 @@
   </si>
   <si>
     <t>EA-EACH</t>
+  </si>
+  <si>
+    <t>selectUOM</t>
+  </si>
+  <si>
+    <t>CU-CUBIC</t>
   </si>
 </sst>
 </file>
@@ -894,7 +901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -976,12 +983,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1. Updated the catalog sheets for 'AddPriceAgrmnt_RecentOrder' and'AddPriceAgrmnt_LocalCatalog'. 2. Updated the test class TC_07 with datasheet name.
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/Catalog.xlsx
+++ b/src/test/resources/datasheets/Catalog.xlsx
@@ -8,15 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="SmartForm" sheetId="1" r:id="rId1"/>
-    <sheet name="AddPriceAgreement" sheetId="2" r:id="rId2"/>
+    <sheet name="AddPriceAgrmnt_RecentOrder" sheetId="2" r:id="rId2"/>
+    <sheet name="AddPriceAgrmnt_LocalCatalog" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Role</t>
   </si>
@@ -27,15 +27,9 @@
     <t xml:space="preserve">Location                      </t>
   </si>
   <si>
-    <t>XEEVA</t>
-  </si>
-  <si>
     <t xml:space="preserve">selectUOM </t>
   </si>
   <si>
-    <t xml:space="preserve">CU-CUBIC </t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -100,6 +94,9 @@
   </si>
   <si>
     <t>EA-EACH</t>
+  </si>
+  <si>
+    <t>CU-CUBIC</t>
   </si>
 </sst>
 </file>
@@ -949,40 +946,40 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -990,37 +987,37 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -1036,7 +1033,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1054,7 +1051,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1062,13 +1059,27 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated existing sheet with new data
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/Catalog.xlsx
+++ b/src/test/resources/datasheets/Catalog.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14985" windowHeight="6210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14985" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="SmartForm" sheetId="1" r:id="rId1"/>
     <sheet name="VerifyCatalogSearch" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1:G19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Role</t>
   </si>
@@ -50,9 +51,6 @@
     <t xml:space="preserve">Price </t>
   </si>
   <si>
-    <t xml:space="preserve">Test Item </t>
-  </si>
-  <si>
     <t>INFORMATION TECHNOLOGY</t>
   </si>
   <si>
@@ -62,9 +60,6 @@
     <t>CELL PHONES</t>
   </si>
   <si>
-    <t>EA-EACH</t>
-  </si>
-  <si>
     <t xml:space="preserve">CatalogSearchInput </t>
   </si>
   <si>
@@ -90,6 +85,42 @@
   </si>
   <si>
     <t>bpo</t>
+  </si>
+  <si>
+    <t>REPOFLOR 100 MG</t>
+  </si>
+  <si>
+    <t>UNSPSC Code</t>
+  </si>
+  <si>
+    <t>UNSPSC001</t>
+  </si>
+  <si>
+    <t>Suggested Supplier(s)</t>
+  </si>
+  <si>
+    <t>Sachin Supplier Magna</t>
+  </si>
+  <si>
+    <t>Manufacturer Name</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number</t>
+  </si>
+  <si>
+    <t>ARMSTRONG</t>
+  </si>
+  <si>
+    <t>MPN001</t>
+  </si>
+  <si>
+    <t>1;10</t>
+  </si>
+  <si>
+    <t>EA-EACH;CU-CUBIC</t>
+  </si>
+  <si>
+    <t>1;2</t>
   </si>
 </sst>
 </file>
@@ -919,26 +950,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="33" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="10" width="20.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -949,25 +981,37 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -975,25 +1019,37 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1005,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1027,16 +1083,16 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1044,19 +1100,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Added the new test data in the catalog sheets - 'AddPriceAgrmnt_FavFolder' & 'AddPriceAgrmnt_LocalCatalog'.
2.Developed a new page class - CartInformationPage.
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/Catalog.xlsx
+++ b/src/test/resources/datasheets/Catalog.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="4230" windowWidth="19320" windowHeight="6015" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="4230" windowWidth="19320" windowHeight="6015" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SmartForm" sheetId="1" r:id="rId1"/>
     <sheet name="AddPriceAgrmnt_RecentOrder" sheetId="2" r:id="rId2"/>
     <sheet name="AddPriceAgrmnt_LocalCatalog" sheetId="3" r:id="rId3"/>
+    <sheet name="AddPriceAgrmnt_FavFolder" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Role</t>
   </si>
@@ -97,6 +98,18 @@
   </si>
   <si>
     <t>CU-CUBIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ItemType </t>
+  </si>
+  <si>
+    <t>ItemNumber</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>156001-00013</t>
   </si>
 </sst>
 </file>
@@ -1032,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1072,14 +1085,83 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated sheet - AddPriceAgrmnt_RecentOrder
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/Catalog.xlsx
+++ b/src/test/resources/datasheets/Catalog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14985" windowHeight="6210"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15825" windowHeight="6210" tabRatio="666" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SmartForm" sheetId="1" r:id="rId1"/>
@@ -13,11 +13,12 @@
     <sheet name="AddPriceAgrmnt_LocalCatalog" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1:N19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Role</t>
   </si>
@@ -140,6 +141,27 @@
   </si>
   <si>
     <t>156001-00013</t>
+  </si>
+  <si>
+    <t>NPAI</t>
+  </si>
+  <si>
+    <t>PAItem</t>
+  </si>
+  <si>
+    <t>NPAItem</t>
+  </si>
+  <si>
+    <t>PAI</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>Qty</t>
   </si>
 </sst>
 </file>
@@ -971,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1141,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1152,9 +1174,10 @@
     <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1164,8 +1187,23 @@
       <c r="C1" t="s">
         <v>36</v>
       </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1174,6 +1212,21 @@
       </c>
       <c r="C2" t="s">
         <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the following tests in catalog Module: 1.Add_PriceAgreement_FavouriteFolder. 2.Add_PriceAgreement_RecentFolder, and 3.Add_PriceAgreement_LocalCatalog.
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/Catalog.xlsx
+++ b/src/test/resources/datasheets/Catalog.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15825" windowHeight="6210" tabRatio="666" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2850" windowWidth="12345" windowHeight="4335" tabRatio="666" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SmartForm" sheetId="1" r:id="rId1"/>
     <sheet name="VerifyCatalogSearch" sheetId="2" r:id="rId2"/>
     <sheet name="AddPriceAgrmnt_RecentOrder" sheetId="3" r:id="rId3"/>
     <sheet name="AddPriceAgrmnt_LocalCatalog" sheetId="4" r:id="rId4"/>
+    <sheet name="AddPriceAgrmnt_FavFolder" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>Role</t>
   </si>
@@ -152,6 +153,15 @@
   </si>
   <si>
     <t>PAI</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>Qty</t>
   </si>
 </sst>
 </file>
@@ -983,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1153,21 +1163,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="2" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1175,7 +1187,7 @@
         <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
         <v>42</v>
@@ -1183,8 +1195,17 @@
       <c r="E1" t="s">
         <v>43</v>
       </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1192,13 +1213,22 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
         <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1210,12 +1240,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1250,4 +1283,46 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Developed new Test "AddNonPriceAgreementItem_FromGlobalItems"
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/Catalog.xlsx
+++ b/src/test/resources/datasheets/Catalog.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15825" windowHeight="6210" tabRatio="666"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15825" windowHeight="6210" tabRatio="666" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SmartForm" sheetId="1" r:id="rId1"/>
     <sheet name="VerifyCatalogSearch" sheetId="2" r:id="rId2"/>
     <sheet name="AddPriceAgrmnt_RecentOrder" sheetId="3" r:id="rId3"/>
     <sheet name="AddPriceAgrmnt_LocalCatalog" sheetId="4" r:id="rId4"/>
+    <sheet name="AddNonPriceAgr_GlobalCatalog" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:G19"/>
+  <oleSize ref="A1:I19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t>Role</t>
   </si>
@@ -162,6 +163,30 @@
   </si>
   <si>
     <t>Qty</t>
+  </si>
+  <si>
+    <t>Global Item</t>
+  </si>
+  <si>
+    <t>ItemDescription</t>
+  </si>
+  <si>
+    <t>UnitPrice</t>
+  </si>
+  <si>
+    <t>UpdatedUnitPrice</t>
+  </si>
+  <si>
+    <t>UpdatedUnitofMeasure</t>
+  </si>
+  <si>
+    <t>Iphone</t>
+  </si>
+  <si>
+    <t>iPhone_d_99_4</t>
+  </si>
+  <si>
+    <t>EA-EACH</t>
   </si>
 </sst>
 </file>
@@ -993,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1103,7 +1128,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1166,7 +1191,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1239,7 +1264,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1275,4 +1300,87 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Pushing line endings to changes.
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/Catalog.xlsx
+++ b/src/test/resources/datasheets/Catalog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15825" windowHeight="6210" tabRatio="666" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15825" windowHeight="6210" tabRatio="666" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="SmartForm" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="AddPriceAgrmnt_RecentOrder" sheetId="3" r:id="rId3"/>
     <sheet name="AddPriceAgrmnt_LocalCatalog" sheetId="4" r:id="rId4"/>
     <sheet name="AddNonPriceAgr_GlobalCatalog" sheetId="5" r:id="rId5"/>
+    <sheet name="AddPriceAgrmnt_FavFolder" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t>Role</t>
   </si>
@@ -1305,7 +1306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -1382,4 +1383,45 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated methodNames, Uncommented driver quit
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/Catalog.xlsx
+++ b/src/test/resources/datasheets/Catalog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15825" windowHeight="6210" tabRatio="666" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16050" windowHeight="6210" tabRatio="666" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SmartForm" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="AddPriceAgrmnt_FavFolder" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1:J19"/>
 </workbook>
 </file>
 
@@ -1204,7 +1205,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1319,7 +1320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -1402,7 +1403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
1. Developed a new test in catalog module - Add_PriceAgreementItem_FromComparisonScreen.
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/Catalog.xlsx
+++ b/src/test/resources/datasheets/Catalog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14895" windowHeight="6210" tabRatio="666" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2850" windowWidth="13935" windowHeight="4170" tabRatio="666" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="SmartForm" sheetId="1" r:id="rId1"/>
@@ -13,14 +13,14 @@
     <sheet name="AddPriceAgrmnt_LocalCatalog" sheetId="4" r:id="rId4"/>
     <sheet name="AddNonPriceAgr_GlobalCatalog" sheetId="5" r:id="rId5"/>
     <sheet name="AddPriceAgrmnt_FavFolder" sheetId="6" r:id="rId6"/>
+    <sheet name="AddPriceAgrmnt_CompareScreen" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <oleSize ref="A1:M19"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
   <si>
     <t>Role</t>
   </si>
@@ -200,6 +200,15 @@
   </si>
   <si>
     <t>selectUOM</t>
+  </si>
+  <si>
+    <t>searchItem</t>
+  </si>
+  <si>
+    <t>UnitofMeasure</t>
+  </si>
+  <si>
+    <t>Iphones</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1321,7 +1330,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1404,7 +1413,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1437,4 +1446,53 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding files to index.
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/Catalog.xlsx
+++ b/src/test/resources/datasheets/Catalog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14895" windowHeight="6210" tabRatio="1000" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14895" windowHeight="6210" tabRatio="1000" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SmartForm" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet name="Verify_AddInternalComments" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:I19"/>
 </workbook>
 </file>
 
@@ -1234,7 +1233,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1306,11 +1305,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1349,7 +1351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -1473,7 +1475,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1519,15 +1521,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1550,7 +1552,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>1</v>
       </c>

</xml_diff>